<commit_message>
Document drafting and advertisement research
</commit_message>
<xml_diff>
--- a/Equity Research Reports/2023Q1 Cruise Lines.xlsx
+++ b/Equity Research Reports/2023Q1 Cruise Lines.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\Equity Research Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458D6DEA-BF01-45B7-AFBE-877573EE2E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8757BEFE-3D1B-47A6-97E5-92376520152B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="31635" windowHeight="21600" activeTab="3" xr2:uid="{1956F853-84B1-49AB-A50B-B169BC564448}"/>
+    <workbookView xWindow="26265" yWindow="0" windowWidth="25335" windowHeight="21600" activeTab="3" xr2:uid="{1956F853-84B1-49AB-A50B-B169BC564448}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Booking Experience" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="7" r:id="rId3"/>
-    <sheet name="Revenues" sheetId="2" r:id="rId4"/>
-    <sheet name="Margins" sheetId="3" r:id="rId5"/>
-    <sheet name="Occupency" sheetId="4" r:id="rId6"/>
-    <sheet name="Debt" sheetId="5" r:id="rId7"/>
+    <sheet name="Booking Cost Compare" sheetId="6" r:id="rId2"/>
+    <sheet name="Booking Experience" sheetId="7" r:id="rId3"/>
+    <sheet name="Advertisements" sheetId="8" r:id="rId4"/>
+    <sheet name="Revenues" sheetId="2" r:id="rId5"/>
+    <sheet name="Margins" sheetId="3" r:id="rId6"/>
+    <sheet name="Occupency" sheetId="4" r:id="rId7"/>
+    <sheet name="Debt" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="224">
   <si>
     <t>Debt maturity schedule</t>
   </si>
@@ -734,6 +735,108 @@
 Choose room location, descriptions on what is nearby
 Insurance and land transport</t>
   </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=hKkO-BIMxtA</t>
+  </si>
+  <si>
+    <t>??? SUCKS WHERE IS UR NAME</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wbp2z_e2r5E</t>
+  </si>
+  <si>
+    <t>15/12/2022</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wvStn8Z7iJU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=hG_vqdVZMyw</t>
+  </si>
+  <si>
+    <t>Meh ad, Where is the sex appeal</t>
+  </si>
+  <si>
+    <t>Good ad</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=gY6kKgY04YY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=6emsasoYPnY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=AoaS7aF0hGU</t>
+  </si>
+  <si>
+    <t>10/10 banger ad</t>
+  </si>
+  <si>
+    <t>Great ad</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=kKxy3zi82AA</t>
+  </si>
+  <si>
+    <t>Friends appeal</t>
+  </si>
+  <si>
+    <t>Broadway style</t>
+  </si>
+  <si>
+    <t>Adventure appeal</t>
+  </si>
+  <si>
+    <t>Adult style</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rqHIjbhx45w</t>
+  </si>
+  <si>
+    <t>Seven seas</t>
+  </si>
+  <si>
+    <t>Travel agents</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=vjGbGHZlf80</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>NCLH caught the cultural zightgeist back in 2014/2015 - knew what they wanted, now a days they are kinda slipping</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ucLwEliJz80</t>
+  </si>
+  <si>
+    <t>Very old style ad. Good ad</t>
+  </si>
+  <si>
+    <t>Old style, stuck in 2010s. Good ad</t>
+  </si>
+  <si>
+    <t>Kid appeal? Family appeal? Idk man</t>
+  </si>
+  <si>
+    <t>Meh ad, but why does the narration make it seem so lame?</t>
+  </si>
+  <si>
+    <t>Good, then bad</t>
+  </si>
+  <si>
+    <t>https://vimeo.com/766715872</t>
+  </si>
+  <si>
+    <t>INVESTOR AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Everyone </t>
+  </si>
+  <si>
+    <t>RCL is absolutely capturing the zoomer/millenial age</t>
+  </si>
 </sst>
 </file>
 
@@ -743,7 +846,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,6 +858,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -777,10 +888,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -806,8 +918,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -952,10 +1067,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Revenues!$B$9:$O$9</c:f>
+              <c:f>Revenues!$B$9:$X$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -997,16 +1112,43 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2032</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Revenues!$B$10:$O$10</c:f>
+              <c:f>Revenues!$B$10:$X$10</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>-0.15168482016105722</c:v>
                 </c:pt>
@@ -1048,6 +1190,33 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.42253271833119688</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.68555603735456083</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.73443716243784296</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.80381464893535681</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.87596723489277095</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.93224625193955424</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99021363949774077</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.0499200486826732</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1114176501431534</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.1747601796474476</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1097,10 +1266,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Revenues!$B$9:$O$9</c:f>
+              <c:f>Revenues!$B$9:$X$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -1142,16 +1311,43 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2032</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Revenues!$B$11:$O$11</c:f>
+              <c:f>Revenues!$B$11:$X$11</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>-6.939525121343304E-2</c:v>
                 </c:pt>
@@ -1193,6 +1389,33 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>9.9421553514165373E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.40066653612448699</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.70191151873480884</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.7699879794842015</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.8407874986635695</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.89601112362347646</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95289145733218072</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.0114782010521464</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.0718225470837108</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.1339772234962222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1242,10 +1465,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Revenues!$B$9:$O$9</c:f>
+              <c:f>Revenues!$B$9:$X$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -1287,16 +1510,43 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2032</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Revenues!$B$12:$O$12</c:f>
+              <c:f>Revenues!$B$12:$X$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>-0.21717918391484337</c:v>
                 </c:pt>
@@ -1338,6 +1588,33 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1.3255510495828347</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.7291052271808582</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.1326594047788814</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.320618969065614</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.486649917518895</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.6261159142196506</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.7711605507884371</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.9220069728199749</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.0788872517327741</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.2420427418020852</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1387,10 +1664,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Revenues!$B$9:$O$9</c:f>
+              <c:f>Revenues!$B$9:$X$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -1432,16 +1709,43 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2032</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Revenues!$B$13:$O$13</c:f>
+              <c:f>Revenues!$B$13:$X$13</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1482,6 +1786,33 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4057,6 +4388,7 @@
         <c:axId val="906688240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="160"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -13727,6 +14059,7 @@
         <c:axId val="386917280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="450"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -15506,6 +15839,7 @@
         <c:axId val="892424144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="400"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -16207,6 +16541,7 @@
         <c:axId val="892414992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="300"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -31588,7 +31923,7 @@
   <dimension ref="B2:U26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31978,10 +32313,10 @@
   <dimension ref="B3:I17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32268,11 +32603,259 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E5DE94-82E3-4824-AA4A-B109D2A61AFA}">
+  <dimension ref="B2:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="16">
+        <v>44936</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="16">
+        <v>44944</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="16">
+        <v>44944</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="16">
+        <v>44854</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="E8" t="s">
+        <v>201</v>
+      </c>
+      <c r="F8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="16">
+        <v>44885</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="16">
+        <v>44956</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E10" t="s">
+        <v>202</v>
+      </c>
+      <c r="F10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="16">
+        <v>44867</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="E11" t="s">
+        <v>221</v>
+      </c>
+      <c r="F11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="16">
+        <v>44803</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E13" t="s">
+        <v>197</v>
+      </c>
+      <c r="F13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>209</v>
+      </c>
+      <c r="C14" s="16">
+        <v>44950</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="E14" t="s">
+        <v>215</v>
+      </c>
+      <c r="F14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="16">
+        <v>43783</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="E15" t="s">
+        <v>202</v>
+      </c>
+      <c r="F15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="16">
+        <v>44524</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="E16" t="s">
+        <v>219</v>
+      </c>
+      <c r="F16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{B330BE20-7644-453A-A380-B11B5007F9FF}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{E6E9CE6A-75BE-46A8-9863-A53470318F93}"/>
+    <hyperlink ref="D9" r:id="rId3" xr:uid="{66F51000-1281-4BA0-8663-59A2043F41AC}"/>
+    <hyperlink ref="D10" r:id="rId4" xr:uid="{3EFBCE2B-B4EB-4410-8C7B-C672ADF7BD49}"/>
+    <hyperlink ref="D15" r:id="rId5" xr:uid="{29BE3035-D420-4196-9C3F-0D062AC55E86}"/>
+    <hyperlink ref="D13" r:id="rId6" xr:uid="{135F5DF0-1374-4A70-AB6A-5F613AE20F22}"/>
+    <hyperlink ref="D14" r:id="rId7" xr:uid="{DBB0F122-D81D-4B4C-A05B-A274DA918618}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{C683AD3D-A7A7-4136-869B-01281836DC5E}"/>
+    <hyperlink ref="D5" r:id="rId9" xr:uid="{B7EA6AD3-5DF6-459B-9529-4E0F77447A5A}"/>
+    <hyperlink ref="D6" r:id="rId10" xr:uid="{8CC98FF6-3815-4345-BB10-0E85F4FB3891}"/>
+    <hyperlink ref="D16" r:id="rId11" xr:uid="{8CBD26AF-7D86-4D94-8045-1D559769104B}"/>
+    <hyperlink ref="D11" r:id="rId12" xr:uid="{FF00683F-8832-4696-A9FD-2D2493915A73}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0658E1-7504-491D-8DCB-12912983ABE7}">
   <dimension ref="A1:X82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W40" sqref="W40"/>
+    <sheetView topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AP46" sqref="AP46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35291,12 +35874,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAFBF3D4-D9EF-4978-A7C8-5C4C5D3FD005}">
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Z13" sqref="Z13"/>
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35896,12 +36479,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1AEFB0-127A-45E7-BA20-B0A55F5C5512}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D10"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="O62" sqref="O62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36975,17 +37558,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047DFB78-7EAE-4E9E-A61F-4F339F29960C}">
   <dimension ref="B3:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="C16" sqref="C16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="6" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>